<commit_message>
more test results :D
</commit_message>
<xml_diff>
--- a/5MTests/5MeterTests.xlsx
+++ b/5MTests/5MeterTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KholySa\OneDrive\Documents\HS Osnabruck\Tests\5MTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4FA600-56F2-46CE-8481-7F02F2BB7583}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B3D87F-32FA-454D-A465-B80C7B934DC2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -564,30 +564,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -609,6 +585,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -926,7 +926,7 @@
   <dimension ref="B1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="B29" sqref="B1:M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -948,29 +948,29 @@
   <sheetData>
     <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20" t="s">
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="21" t="s">
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="39" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="19"/>
+      <c r="B3" s="37"/>
       <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1001,180 +1001,180 @@
       <c r="L3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="22"/>
+      <c r="M3" s="40"/>
     </row>
     <row r="4" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="17"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="43"/>
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="16">
         <v>18</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="16">
         <v>-30</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="16">
         <v>22</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="16">
         <v>30</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="17">
         <v>12</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="16">
         <v>22</v>
       </c>
-      <c r="I5" s="24">
+      <c r="I5" s="16">
         <v>0</v>
       </c>
-      <c r="J5" s="24">
+      <c r="J5" s="16">
         <v>17</v>
       </c>
-      <c r="K5" s="24">
+      <c r="K5" s="16">
         <v>-5</v>
       </c>
-      <c r="L5" s="24">
+      <c r="L5" s="16">
         <v>5</v>
       </c>
-      <c r="M5" s="26"/>
+      <c r="M5" s="18"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="28">
+      <c r="C6" s="20">
         <v>-75</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="20">
         <v>-176</v>
       </c>
-      <c r="E6" s="28">
+      <c r="E6" s="20">
         <v>-149</v>
       </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="29">
+      <c r="F6" s="20"/>
+      <c r="G6" s="21">
         <v>-80</v>
       </c>
-      <c r="H6" s="28">
+      <c r="H6" s="20">
         <v>-108</v>
       </c>
-      <c r="I6" s="28">
+      <c r="I6" s="20">
         <v>-141</v>
       </c>
-      <c r="J6" s="28">
+      <c r="J6" s="20">
         <v>-136</v>
       </c>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28">
+      <c r="K6" s="20"/>
+      <c r="L6" s="20">
         <v>-110</v>
       </c>
-      <c r="M6" s="30"/>
+      <c r="M6" s="22"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="20">
         <v>86</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="20">
         <v>41</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="20">
         <v>53</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="20">
         <v>58</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="21">
         <v>29</v>
       </c>
-      <c r="H7" s="28">
+      <c r="H7" s="20">
         <v>-46</v>
       </c>
-      <c r="I7" s="28">
+      <c r="I7" s="20">
         <v>-37</v>
       </c>
-      <c r="J7" s="28">
+      <c r="J7" s="20">
         <v>-40</v>
       </c>
-      <c r="K7" s="28">
+      <c r="K7" s="20">
         <v>-55</v>
       </c>
-      <c r="L7" s="28">
+      <c r="L7" s="20">
         <v>-29</v>
       </c>
-      <c r="M7" s="30"/>
+      <c r="M7" s="22"/>
     </row>
     <row r="8" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="24">
         <v>-16</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="24">
         <v>-17</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="24">
         <v>-7</v>
       </c>
-      <c r="F8" s="32">
+      <c r="F8" s="24">
         <v>-41</v>
       </c>
-      <c r="G8" s="33">
+      <c r="G8" s="25">
         <v>8</v>
       </c>
-      <c r="H8" s="32">
+      <c r="H8" s="24">
         <v>-18</v>
       </c>
-      <c r="I8" s="32">
+      <c r="I8" s="24">
         <v>-8</v>
       </c>
-      <c r="J8" s="32">
+      <c r="J8" s="24">
         <v>-41</v>
       </c>
-      <c r="K8" s="32">
+      <c r="K8" s="24">
         <v>3</v>
       </c>
-      <c r="L8" s="32">
+      <c r="L8" s="24">
         <v>-16</v>
       </c>
-      <c r="M8" s="34"/>
+      <c r="M8" s="26"/>
     </row>
     <row r="9" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="17"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="43"/>
     </row>
     <row r="10" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
@@ -1192,10 +1192,10 @@
       <c r="F10" s="4">
         <v>36</v>
       </c>
-      <c r="G10" s="38">
+      <c r="G10" s="30">
         <v>-37</v>
       </c>
-      <c r="H10" s="35">
+      <c r="H10" s="27">
         <v>14</v>
       </c>
       <c r="I10" s="4">
@@ -1228,10 +1228,10 @@
       <c r="F11" s="2">
         <v>14</v>
       </c>
-      <c r="G11" s="39">
+      <c r="G11" s="31">
         <v>-9</v>
       </c>
-      <c r="H11" s="36">
+      <c r="H11" s="28">
         <v>-70</v>
       </c>
       <c r="I11" s="2">
@@ -1264,10 +1264,10 @@
       <c r="F12" s="2">
         <v>-77</v>
       </c>
-      <c r="G12" s="39">
+      <c r="G12" s="31">
         <v>20</v>
       </c>
-      <c r="H12" s="36">
+      <c r="H12" s="28">
         <v>153</v>
       </c>
       <c r="I12" s="2">
@@ -1300,10 +1300,10 @@
       <c r="F13" s="5">
         <v>-2</v>
       </c>
-      <c r="G13" s="40">
+      <c r="G13" s="32">
         <v>-4</v>
       </c>
-      <c r="H13" s="37">
+      <c r="H13" s="29">
         <v>39</v>
       </c>
       <c r="I13" s="5">
@@ -1321,20 +1321,20 @@
       <c r="M13" s="11"/>
     </row>
     <row r="14" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="17"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="43"/>
     </row>
     <row r="15" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
@@ -1352,10 +1352,10 @@
       <c r="F15" s="4">
         <v>-89</v>
       </c>
-      <c r="G15" s="38">
+      <c r="G15" s="30">
         <v>4</v>
       </c>
-      <c r="H15" s="35">
+      <c r="H15" s="27">
         <v>5</v>
       </c>
       <c r="I15" s="4">
@@ -1388,10 +1388,10 @@
       <c r="F16" s="2">
         <v>0</v>
       </c>
-      <c r="G16" s="39">
+      <c r="G16" s="31">
         <v>-43</v>
       </c>
-      <c r="H16" s="36">
+      <c r="H16" s="28">
         <v>-27</v>
       </c>
       <c r="I16" s="2">
@@ -1412,129 +1412,249 @@
       <c r="B17" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
+      <c r="C17" s="2">
+        <v>91</v>
+      </c>
+      <c r="D17" s="2">
+        <v>16</v>
+      </c>
+      <c r="E17" s="2">
+        <v>98</v>
+      </c>
+      <c r="F17" s="2">
+        <v>21</v>
+      </c>
+      <c r="G17" s="31">
+        <v>24</v>
+      </c>
+      <c r="H17" s="28">
+        <v>2</v>
+      </c>
+      <c r="I17" s="2">
+        <v>-8</v>
+      </c>
+      <c r="J17" s="2">
+        <v>-1</v>
+      </c>
+      <c r="K17" s="2">
+        <v>-2</v>
+      </c>
+      <c r="L17" s="2">
+        <v>-15</v>
+      </c>
       <c r="M17" s="9"/>
     </row>
     <row r="18" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
+      <c r="C18" s="5">
+        <v>52</v>
+      </c>
+      <c r="D18" s="5">
+        <v>-16</v>
+      </c>
+      <c r="E18" s="5">
+        <v>17</v>
+      </c>
+      <c r="F18" s="5">
+        <v>-57</v>
+      </c>
+      <c r="G18" s="32">
+        <v>21</v>
+      </c>
+      <c r="H18" s="29">
+        <v>12</v>
+      </c>
+      <c r="I18" s="5">
+        <v>8</v>
+      </c>
+      <c r="J18" s="5">
+        <v>5</v>
+      </c>
+      <c r="K18" s="5">
+        <v>8</v>
+      </c>
+      <c r="L18" s="5">
+        <v>6</v>
+      </c>
       <c r="M18" s="11"/>
     </row>
     <row r="19" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="17"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="42"/>
+      <c r="M19" s="43"/>
     </row>
     <row r="20" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
+      <c r="C20" s="4">
+        <v>-80</v>
+      </c>
+      <c r="D20" s="4">
+        <v>-43</v>
+      </c>
+      <c r="E20" s="4">
+        <v>-80</v>
+      </c>
+      <c r="F20" s="4">
+        <v>-5</v>
+      </c>
+      <c r="G20" s="30">
+        <v>-109</v>
+      </c>
+      <c r="H20" s="27">
+        <v>39</v>
+      </c>
+      <c r="I20" s="4">
+        <v>37</v>
+      </c>
+      <c r="J20" s="4">
+        <v>37</v>
+      </c>
+      <c r="K20" s="4">
+        <v>30</v>
+      </c>
+      <c r="L20" s="4">
+        <v>45</v>
+      </c>
       <c r="M20" s="7"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B21" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
+      <c r="C21" s="2">
+        <v>51</v>
+      </c>
+      <c r="D21" s="2">
+        <v>-53</v>
+      </c>
+      <c r="E21" s="2">
+        <v>12</v>
+      </c>
+      <c r="F21" s="2">
+        <v>-41</v>
+      </c>
+      <c r="G21" s="31">
+        <v>51</v>
+      </c>
+      <c r="H21" s="28">
+        <v>21</v>
+      </c>
+      <c r="I21" s="2">
+        <v>5</v>
+      </c>
+      <c r="J21" s="2">
+        <v>-2</v>
+      </c>
+      <c r="K21" s="2">
+        <v>-16</v>
+      </c>
+      <c r="L21" s="2">
+        <v>16</v>
+      </c>
       <c r="M21" s="9"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B22" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
+      <c r="C22" s="2">
+        <v>100</v>
+      </c>
+      <c r="D22" s="2">
+        <v>6</v>
+      </c>
+      <c r="E22" s="2">
+        <v>114</v>
+      </c>
+      <c r="F22" s="2">
+        <v>-30</v>
+      </c>
+      <c r="G22" s="31">
+        <v>-78</v>
+      </c>
+      <c r="H22" s="28">
+        <v>1</v>
+      </c>
+      <c r="I22" s="2">
+        <v>5</v>
+      </c>
+      <c r="J22" s="2">
+        <v>9</v>
+      </c>
+      <c r="K22" s="2">
+        <v>-9</v>
+      </c>
+      <c r="L22" s="2">
+        <v>15</v>
+      </c>
       <c r="M22" s="9"/>
     </row>
     <row r="23" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
+      <c r="C23" s="5">
+        <v>29</v>
+      </c>
+      <c r="D23" s="5">
+        <v>-51</v>
+      </c>
+      <c r="E23" s="5">
+        <v>22</v>
+      </c>
+      <c r="F23" s="5">
+        <v>-32</v>
+      </c>
+      <c r="G23" s="34">
+        <v>-22</v>
+      </c>
+      <c r="H23" s="29">
+        <v>14</v>
+      </c>
+      <c r="I23" s="5">
+        <v>30</v>
+      </c>
+      <c r="J23" s="5">
+        <v>5</v>
+      </c>
+      <c r="K23" s="5">
+        <v>14</v>
+      </c>
+      <c r="L23" s="5">
+        <v>7</v>
+      </c>
       <c r="M23" s="11"/>
     </row>
     <row r="24" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="17"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="43"/>
     </row>
     <row r="25" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
@@ -1544,8 +1664,8 @@
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="35"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="27"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
@@ -1560,8 +1680,8 @@
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="36"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="28"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
@@ -1576,8 +1696,8 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="36"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="28"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
@@ -1592,8 +1712,8 @@
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="37"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="29"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
@@ -1601,20 +1721,20 @@
       <c r="M28" s="11"/>
     </row>
     <row r="29" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="17"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="42"/>
+      <c r="K29" s="42"/>
+      <c r="L29" s="42"/>
+      <c r="M29" s="43"/>
     </row>
     <row r="30" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B30" s="6" t="s">
@@ -1624,8 +1744,8 @@
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="35"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="27"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
@@ -1640,8 +1760,8 @@
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="36"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="28"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
@@ -1656,8 +1776,8 @@
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="36"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="28"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
@@ -1672,8 +1792,8 @@
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
-      <c r="G33" s="42"/>
-      <c r="H33" s="37"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="29"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
@@ -1681,20 +1801,20 @@
       <c r="M33" s="11"/>
     </row>
     <row r="34" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16"/>
-      <c r="L34" s="16"/>
-      <c r="M34" s="17"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
+      <c r="H34" s="42"/>
+      <c r="I34" s="42"/>
+      <c r="J34" s="42"/>
+      <c r="K34" s="42"/>
+      <c r="L34" s="42"/>
+      <c r="M34" s="43"/>
     </row>
     <row r="35" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B35" s="6" t="s">
@@ -1704,8 +1824,8 @@
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
-      <c r="G35" s="38"/>
-      <c r="H35" s="35"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="27"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
@@ -1720,8 +1840,8 @@
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
-      <c r="G36" s="39"/>
-      <c r="H36" s="36"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="28"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
@@ -1736,8 +1856,8 @@
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
-      <c r="G37" s="39"/>
-      <c r="H37" s="36"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="28"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
@@ -1752,8 +1872,8 @@
       <c r="D38" s="13"/>
       <c r="E38" s="13"/>
       <c r="F38" s="13"/>
-      <c r="G38" s="43"/>
-      <c r="H38" s="41"/>
+      <c r="G38" s="35"/>
+      <c r="H38" s="33"/>
       <c r="I38" s="13"/>
       <c r="J38" s="13"/>
       <c r="K38" s="13"/>
@@ -1762,17 +1882,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="B4:M4"/>
     <mergeCell ref="B34:M34"/>
     <mergeCell ref="B9:M9"/>
     <mergeCell ref="B14:M14"/>
     <mergeCell ref="B19:M19"/>
     <mergeCell ref="B24:M24"/>
     <mergeCell ref="B29:M29"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="B4:M4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>